<commit_message>
JS8_Perbaikan penambahan Export Import & Tugas Upload Profile
</commit_message>
<xml_diff>
--- a/public/template_barang.xlsx
+++ b/public/template_barang.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9390" windowHeight="7650"/>
+    <workbookView windowWidth="19635" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>kategori_id</t>
   </si>
@@ -31,34 +31,10 @@
     <t xml:space="preserve">harga_jual </t>
   </si>
   <si>
-    <t>FUR10</t>
+    <t>ELEK90</t>
   </si>
   <si>
-    <t>Lemari Baju 2 Pintu</t>
-  </si>
-  <si>
-    <t>ELEK01</t>
-  </si>
-  <si>
-    <t>Hair Dryer Dyson</t>
-  </si>
-  <si>
-    <t>ELEK02</t>
-  </si>
-  <si>
-    <t>Vacum Culeaner Polytron</t>
-  </si>
-  <si>
-    <t>BJU01</t>
-  </si>
-  <si>
-    <t>Gamis Muslimah Pink</t>
-  </si>
-  <si>
-    <t>BJU02</t>
-  </si>
-  <si>
-    <t>One set dress floral</t>
+    <t>Mouse Robot</t>
   </si>
 </sst>
 </file>
@@ -1211,13 +1187,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
@@ -1245,7 +1221,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1254,78 +1230,10 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>20000000</v>
+        <v>90000</v>
       </c>
       <c r="E2">
-        <v>25000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>9000000</v>
-      </c>
-      <c r="E3">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>1500000</v>
-      </c>
-      <c r="E4">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
         <v>130000</v>
-      </c>
-      <c r="E5">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>89000</v>
-      </c>
-      <c r="E6">
-        <v>99000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>